<commit_message>
Commit please refer to instructions
</commit_message>
<xml_diff>
--- a/DispatcherDuProject/Data/Config.xlsx
+++ b/DispatcherDuProject/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\UiPath\LinkedIn Projects\Mail Doc Processor Document Understanding\DispatcherDuProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853C1320-D75E-4651-BA8F-5EE5886458C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B66645-E087-499F-82E6-F29AA3FCD6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21585" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>C:\Users\DELL\Documents\UiPath\LinkedIn Projects\Mail Doc Processor Document Understanding\FilesInput</t>
+  </si>
+  <si>
+    <t>Input Files previously downloaded from Outlook</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -631,6 +634,9 @@
       </c>
       <c r="B6" t="s">
         <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>